<commit_message>
Art. -> Art in data Excel sheet
</commit_message>
<xml_diff>
--- a/data_xlsx/PTAn4.xlsx
+++ b/data_xlsx/PTAn4.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maciejuberna/Dev/PTAn/data_xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB71E10-F6E5-E940-987E-67326BA4B276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2277A54-5D4C-AD4B-BBEC-D0D101DC6187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="500" windowWidth="35880" windowHeight="20680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-40" yWindow="500" windowWidth="35880" windowHeight="20680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US2016G1tv_IS_manualPTA" sheetId="6" r:id="rId1"/>
     <sheet name="Climate_PTA" sheetId="7" r:id="rId2"/>
-    <sheet name="Art._PTA" sheetId="8" r:id="rId3"/>
+    <sheet name="Art_PTA" sheetId="8" r:id="rId3"/>
     <sheet name="Tax_PTA" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -20747,8 +20747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DC20F7B-83F4-DD41-83FA-3B1969FE2781}">
   <dimension ref="A1:T138"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -29322,7 +29322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7D0C67-59BC-7B42-9198-EC5B9860EABE}">
   <dimension ref="A1:T216"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>

</xml_diff>